<commit_message>
poprawka swingu, dodanie wydmuchu
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotr\Documents\Visual Studio 2017\Projects\Optimization24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0F27DECB-14D9-4B04-B71D-E1F6B26FCD6F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FF13CF7F-58DC-4210-9CBF-22CA2FFD506E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13515" activeTab="1" xr2:uid="{FC28733D-4F8B-4A78-9EE2-CAB01ED11EF3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13515" activeTab="2" xr2:uid="{FC28733D-4F8B-4A78-9EE2-CAB01ED11EF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Zestaw1" sheetId="1" r:id="rId1"/>
     <sheet name="Zestaw2" sheetId="2" r:id="rId2"/>
+    <sheet name="Zestaw3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
   <si>
     <t>KS4</t>
   </si>
@@ -74,6 +75,27 @@
   </si>
   <si>
     <t>354.7</t>
+  </si>
+  <si>
+    <t>376.7</t>
+  </si>
+  <si>
+    <t>371.5</t>
+  </si>
+  <si>
+    <t>292.5</t>
+  </si>
+  <si>
+    <t>295.7</t>
+  </si>
+  <si>
+    <t>302.6</t>
+  </si>
+  <si>
+    <t>297.4</t>
+  </si>
+  <si>
+    <t>296.1</t>
   </si>
 </sst>
 </file>
@@ -811,7 +833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9544248-C420-4573-9899-2FFF0229DCD9}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -1267,4 +1289,466 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC11148-8B19-41B9-8DCC-132EA3F16E34}">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>99</v>
+      </c>
+      <c r="D2">
+        <v>541</v>
+      </c>
+      <c r="E2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>45</v>
+      </c>
+      <c r="C3">
+        <v>99</v>
+      </c>
+      <c r="D3">
+        <v>551</v>
+      </c>
+      <c r="E3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>45</v>
+      </c>
+      <c r="C4">
+        <v>99</v>
+      </c>
+      <c r="D4">
+        <v>551</v>
+      </c>
+      <c r="E4">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>45</v>
+      </c>
+      <c r="C5">
+        <v>99</v>
+      </c>
+      <c r="D5">
+        <v>549</v>
+      </c>
+      <c r="E5">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>375</v>
+      </c>
+      <c r="B6">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>99</v>
+      </c>
+      <c r="D6">
+        <v>547</v>
+      </c>
+      <c r="E6">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>46</v>
+      </c>
+      <c r="C7">
+        <v>97</v>
+      </c>
+      <c r="D7">
+        <v>530</v>
+      </c>
+      <c r="E7">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>531</v>
+      </c>
+      <c r="E8">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>102</v>
+      </c>
+      <c r="D9">
+        <v>536</v>
+      </c>
+      <c r="E9">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>45</v>
+      </c>
+      <c r="C10">
+        <v>86</v>
+      </c>
+      <c r="D10">
+        <v>509</v>
+      </c>
+      <c r="E10">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <v>86</v>
+      </c>
+      <c r="D11">
+        <v>509</v>
+      </c>
+      <c r="E11">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>45</v>
+      </c>
+      <c r="C12">
+        <v>86</v>
+      </c>
+      <c r="D12">
+        <v>509</v>
+      </c>
+      <c r="E12">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>45</v>
+      </c>
+      <c r="C13">
+        <v>86</v>
+      </c>
+      <c r="D13">
+        <v>509</v>
+      </c>
+      <c r="E13">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>45</v>
+      </c>
+      <c r="C14">
+        <v>86</v>
+      </c>
+      <c r="D14">
+        <v>508</v>
+      </c>
+      <c r="E14">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>45</v>
+      </c>
+      <c r="C15">
+        <v>86</v>
+      </c>
+      <c r="D15">
+        <v>511</v>
+      </c>
+      <c r="E15">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>45</v>
+      </c>
+      <c r="C16">
+        <v>89</v>
+      </c>
+      <c r="D16">
+        <v>512</v>
+      </c>
+      <c r="E16">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>46</v>
+      </c>
+      <c r="C17">
+        <v>92</v>
+      </c>
+      <c r="D17">
+        <v>518</v>
+      </c>
+      <c r="E17">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>45</v>
+      </c>
+      <c r="C18">
+        <v>87</v>
+      </c>
+      <c r="D18">
+        <v>512</v>
+      </c>
+      <c r="E18">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>45</v>
+      </c>
+      <c r="C19">
+        <v>87</v>
+      </c>
+      <c r="D19">
+        <v>508</v>
+      </c>
+      <c r="E19">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>45</v>
+      </c>
+      <c r="C20">
+        <v>87</v>
+      </c>
+      <c r="D20">
+        <v>508</v>
+      </c>
+      <c r="E20">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>45</v>
+      </c>
+      <c r="C21">
+        <v>87</v>
+      </c>
+      <c r="D21">
+        <v>508</v>
+      </c>
+      <c r="E21">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>45</v>
+      </c>
+      <c r="C22">
+        <v>87</v>
+      </c>
+      <c r="D22">
+        <v>508</v>
+      </c>
+      <c r="E22">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>45</v>
+      </c>
+      <c r="C23">
+        <v>87</v>
+      </c>
+      <c r="D23">
+        <v>508</v>
+      </c>
+      <c r="E23">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>45</v>
+      </c>
+      <c r="C24">
+        <v>90</v>
+      </c>
+      <c r="D24">
+        <v>508</v>
+      </c>
+      <c r="E24">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>45</v>
+      </c>
+      <c r="C25">
+        <v>92</v>
+      </c>
+      <c r="D25">
+        <v>517</v>
+      </c>
+      <c r="E25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>_xlfn.CONCAT("c(",A2,",",A3,",",A4,",",A5,",",A6,",",A7,",",A8,",",A9,",",A10,",",A11,",",A12,",",A13,",",A14,",",A15,",",A16,",",A17,",",A18,",",A19,",",A20,",",A21,",",A22,",",A23,",",A24,",",A25,")")</f>
+        <v>c(376.7,376.7,376.7,376.7,375,371.5,371.5,371.5,292.5,292.5,292.5,292.5,292.5,295.7,295.7,302.6,297.4,296.1,296.1,296.1,296.1,296.1,296.1,296.1)</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" ref="B26:E26" si="0">_xlfn.CONCAT("c(",B2,",",B3,",",B4,",",B5,",",B6,",",B7,",",B8,",",B9,",",B10,",",B11,",",B12,",",B13,",",B14,",",B15,",",B16,",",B17,",",B18,",",B19,",",B20,",",B21,",",B22,",",B23,",",B24,",",B25,")")</f>
+        <v>c(45,45,45,45,46,46,45,46,45,45,45,45,45,45,45,46,45,45,45,45,45,45,45,45)</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>c(99,99,99,99,99,97,100,102,86,86,86,86,86,86,89,92,87,87,87,87,87,87,90,92)</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>c(541,551,551,549,547,530,531,536,509,509,509,509,508,511,512,518,512,508,508,508,508,508,508,517)</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>c(141,144,144,144,143,139,139,139,129,129,129,129,129,130,130,132,131,130,130,128,130,130,130,134)</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>